<commit_message>
add score excel pages
Signed-off-by: yangjiawei <yangjiawei@xiaomi.com>
</commit_message>
<xml_diff>
--- a/resource/reports/teamScores/2017autumn_team_score_list.xlsx
+++ b/resource/reports/teamScores/2017autumn_team_score_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>团队id</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>test tean 1</t>
+  </si>
+  <si>
+    <t>团队1</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,7 +391,18 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>